<commit_message>
done all test cases
</commit_message>
<xml_diff>
--- a/src/com/selenium/testdata/LoginData.xlsx
+++ b/src/com/selenium/testdata/LoginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sudipa chandra\repo\SimpliLearnSeleniumAssessment\src\com\selenium\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE52F6C7-34CF-4B5D-8682-B935969296DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D534912-6D8E-4B50-A8E7-ED1508600FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>sriyansh@csn.com</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>The dress is nice.Quality is perferct as fer expectation.</t>
+  </si>
+  <si>
+    <t>googleEmail</t>
+  </si>
+  <si>
+    <t>ritu@csn.com</t>
   </si>
 </sst>
 </file>
@@ -406,33 +412,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AC501B-C3F9-483E-8E54-5AD596D9B44E}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{5A72E1A5-2FCB-45B3-A530-8CF2136EE74A}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{AAD00DA2-327E-4E93-9878-247E72FC0B5A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -557,7 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12AD6909-6E49-42FE-A4CB-690386B2617E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modified some file for create account
</commit_message>
<xml_diff>
--- a/src/com/selenium/testdata/LoginData.xlsx
+++ b/src/com/selenium/testdata/LoginData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sudipa chandra\repo\SimpliLearnSeleniumAssessment\src\com\selenium\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D534912-6D8E-4B50-A8E7-ED1508600FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D630D735-98B7-4963-8C85-B7F3BE2277B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="CreateAccount" sheetId="9" r:id="rId2"/>
     <sheet name="InvalidData" sheetId="2" r:id="rId3"/>
     <sheet name="SearchValue" sheetId="3" r:id="rId4"/>
     <sheet name="SearchData" sheetId="4" r:id="rId5"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>sriyansh@csn.com</t>
   </si>
@@ -84,6 +84,90 @@
   </si>
   <si>
     <t>ritu@csn.com</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>address1</t>
+  </si>
+  <si>
+    <t>address2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>phno</t>
+  </si>
+  <si>
+    <t>alias</t>
+  </si>
+  <si>
+    <t>sriyansh</t>
+  </si>
+  <si>
+    <t>roy</t>
+  </si>
+  <si>
+    <t>sudipa123</t>
+  </si>
+  <si>
+    <t>reliance</t>
+  </si>
+  <si>
+    <t>bangalore,hsr</t>
+  </si>
+  <si>
+    <t>creative apartment</t>
+  </si>
+  <si>
+    <t>bangalore</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>9898989898</t>
+  </si>
+  <si>
+    <t>00000</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -128,9 +212,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -414,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AC501B-C3F9-483E-8E54-5AD596D9B44E}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -452,13 +537,121 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E56BBA4-4232-4B7F-83B9-D1CB27743458}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B80C1D-1BCF-4024-BE0A-EF5C4729ED59}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>